<commit_message>
delete old and update
</commit_message>
<xml_diff>
--- a/spp3.xlsx
+++ b/spp3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18468" windowHeight="9420"/>
+    <workbookView windowWidth="22368" windowHeight="9420"/>
   </bookViews>
   <sheets>
     <sheet name="Relu" sheetId="2" r:id="rId1"/>
@@ -1152,7 +1152,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="O2" sqref="O2:O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>